<commit_message>
Make new test generate valid MODS
</commit_message>
<xml_diff>
--- a/spec/fixtures/origin-info-update.xlsx
+++ b/spec/fixtures/origin-info-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\arcadia\GitHub\modsulator-app-rails\spec\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAE767C1-792B-44F4-97E0-048C25A2E376}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF2DF9-CB25-47B6-81AC-AE03E66B3E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6CF9945-49E1-4734-B213-29768B403B37}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Identification</t>
   </si>
@@ -177,15 +177,6 @@
     <t>aaa</t>
   </si>
   <si>
-    <t>marccountry-a</t>
-  </si>
-  <si>
-    <t>http://marccountry-a.org/</t>
-  </si>
-  <si>
-    <t>http://marccountry-a.org/aaa</t>
-  </si>
-  <si>
     <t>San Francisco</t>
   </si>
   <si>
@@ -196,15 +187,6 @@
   </si>
   <si>
     <t>bbb</t>
-  </si>
-  <si>
-    <t>marccountry-b</t>
-  </si>
-  <si>
-    <t>http://marccountry-b.org/</t>
-  </si>
-  <si>
-    <t>http://marccountry-b.org/bbb</t>
   </si>
   <si>
     <t>Oakland</t>
@@ -222,15 +204,6 @@
     <t>pub</t>
   </si>
   <si>
-    <t>marccountry-pub</t>
-  </si>
-  <si>
-    <t>http://marccountry-pub.org</t>
-  </si>
-  <si>
-    <t>http://marccountry-pub.org/pub</t>
-  </si>
-  <si>
     <t>London</t>
   </si>
   <si>
@@ -241,15 +214,6 @@
   </si>
   <si>
     <t>production</t>
-  </si>
-  <si>
-    <t>marccountry-pro</t>
-  </si>
-  <si>
-    <t>http://marccountry-pro.org/</t>
-  </si>
-  <si>
-    <t>http://marccountry-pro.org/pro</t>
   </si>
   <si>
     <t>pro</t>
@@ -270,15 +234,6 @@
     <t>dis</t>
   </si>
   <si>
-    <t>marccountry-dis</t>
-  </si>
-  <si>
-    <t>http://marccountry-dis.org/</t>
-  </si>
-  <si>
-    <t>http://marccountry-dis.org/dis</t>
-  </si>
-  <si>
     <t>Tokyo</t>
   </si>
   <si>
@@ -286,6 +241,39 @@
   </si>
   <si>
     <t>http://naf-tok.org/tok</t>
+  </si>
+  <si>
+    <t>marccountry</t>
+  </si>
+  <si>
+    <t>marcgac</t>
+  </si>
+  <si>
+    <t>http://marccountry.org/</t>
+  </si>
+  <si>
+    <t>http://marccountry.org/aaa</t>
+  </si>
+  <si>
+    <t>http://marcgac.org/</t>
+  </si>
+  <si>
+    <t>http://marcgac.org/bbb</t>
+  </si>
+  <si>
+    <t>iso3166</t>
+  </si>
+  <si>
+    <t>http://iso3166.org/</t>
+  </si>
+  <si>
+    <t>http://iso3166.org/pub</t>
+  </si>
+  <si>
+    <t>http://marccountry.org/pro</t>
+  </si>
+  <si>
+    <t>http://marcgac.org/dis</t>
   </si>
 </sst>
 </file>
@@ -720,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0977BA8B-1F79-4415-9103-89020C400504}">
   <dimension ref="A1:AP999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,7 +907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>44</v>
       </c>
@@ -932,115 +920,115 @@
         <v>46</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="M3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="R3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="T3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="U3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Y3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="AA3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="AC3" s="5" t="s">
         <v>69</v>
       </c>
       <c r="AD3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AE3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AL3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AG3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL3" s="9" t="s">
+      <c r="AM3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AM3" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="AN3" s="5" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="AO3" s="9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="AP3" s="9" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.35">
@@ -44887,6 +44875,8 @@
     <hyperlink ref="AM3" r:id="rId16" xr:uid="{57A0DE80-A42A-45FB-9A99-2AF30C5855E6}"/>
     <hyperlink ref="AO3" r:id="rId17" xr:uid="{46DF1A6D-4A1E-4B44-B185-DCD6B5B678DF}"/>
     <hyperlink ref="AP3" r:id="rId18" xr:uid="{D82B7367-282C-4C32-8032-A0FD6C8E93E4}"/>
+    <hyperlink ref="AD3" r:id="rId19" xr:uid="{4FDC071E-027B-41EE-9F38-399734F1FB4A}"/>
+    <hyperlink ref="AE3" r:id="rId20" xr:uid="{75AF487E-D69F-490F-964B-9830285BD33F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>